<commit_message>
add test case for drug page
</commit_message>
<xml_diff>
--- a/MTP_TEST_SHEET/test_cases.xlsx
+++ b/MTP_TEST_SHEET/test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheny39/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheny39/Documents/work/mtp/tmp/ccdi-mtp-visual-testing-katalon/MTP_TEST_SHEET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE785F92-56CE-3D49-978D-5D4E1C1BBFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FF4A3C-24F2-8A4F-A7D2-BF0210795B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="1780" windowWidth="21300" windowHeight="14440" xr2:uid="{4CA04EDA-5F88-F44F-AED6-BB3F5A70B725}"/>
+    <workbookView xWindow="6400" yWindow="1780" windowWidth="14900" windowHeight="14440" xr2:uid="{4CA04EDA-5F88-F44F-AED6-BB3F5A70B725}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="224">
   <si>
     <t>suffixUrl</t>
   </si>
@@ -651,6 +651,63 @@
   </si>
   <si>
     <t>evidence_Orphanet_98657_ENSG00000112715</t>
+  </si>
+  <si>
+    <t>https://ccdi-opentargets-dev.bento-tools.org</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL818</t>
+  </si>
+  <si>
+    <t>drug_IOBENGUANE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL44657</t>
+  </si>
+  <si>
+    <t>drug_ETOPOSIDE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL1200645</t>
+  </si>
+  <si>
+    <t>drug_ETOPOSIDE_PHOSPHATE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL635</t>
+  </si>
+  <si>
+    <t>drug_PREDNISONE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL1201610</t>
+  </si>
+  <si>
+    <t>drug_CORTICOTROPIN</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL501867</t>
+  </si>
+  <si>
+    <t>drug_VINCRISTINE_SULFATE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL359744</t>
+  </si>
+  <si>
+    <t>drug_DOXORUBICIN _HYDROCHLORIDE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL90555</t>
+  </si>
+  <si>
+    <t>drug_VINCRISTINE</t>
+  </si>
+  <si>
+    <t>/drug/CHEMBL1201670</t>
+  </si>
+  <si>
+    <t>drug_SARGRAMOSTIM</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8D0294-7B17-C346-9BB8-48947A2F0825}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2399,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>83</v>
       </c>
@@ -2413,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>83</v>
       </c>
@@ -2427,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>83</v>
       </c>
@@ -2441,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>83</v>
       </c>
@@ -2455,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>83</v>
       </c>
@@ -2467,6 +2524,108 @@
       </c>
       <c r="D101">
         <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102" t="s">
+        <v>206</v>
+      </c>
+      <c r="C102" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B103" t="s">
+        <v>208</v>
+      </c>
+      <c r="C103" t="s">
+        <v>209</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" t="s">
+        <v>210</v>
+      </c>
+      <c r="C104" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" t="s">
+        <v>212</v>
+      </c>
+      <c r="C105" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B106" t="s">
+        <v>214</v>
+      </c>
+      <c r="C106" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" t="s">
+        <v>216</v>
+      </c>
+      <c r="C107" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B108" t="s">
+        <v>218</v>
+      </c>
+      <c r="C108" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B109" t="s">
+        <v>220</v>
+      </c>
+      <c r="C109" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B110" t="s">
+        <v>222</v>
+      </c>
+      <c r="C110" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2572,6 +2731,15 @@
     <hyperlink ref="A92" r:id="rId98" xr:uid="{A251DCE1-A218-9C42-A091-1EBDCB322C8A}"/>
     <hyperlink ref="A94" r:id="rId99" xr:uid="{E192E3D8-CDF6-9A41-8FBE-217E952F178A}"/>
     <hyperlink ref="A96" r:id="rId100" xr:uid="{422FACDF-39FD-494B-B5E6-865160AB2945}"/>
+    <hyperlink ref="A103" r:id="rId101" xr:uid="{5FAFFCE1-3385-0646-A1B3-A52EAA0F579E}"/>
+    <hyperlink ref="A105" r:id="rId102" xr:uid="{55960144-4B5A-DC47-AB53-27BF74175BAF}"/>
+    <hyperlink ref="A107" r:id="rId103" xr:uid="{CFA1B38F-99F2-1640-B61D-733691B78337}"/>
+    <hyperlink ref="A109" r:id="rId104" xr:uid="{1F02CAA5-DCD4-A149-B3BD-078CBA5D18C6}"/>
+    <hyperlink ref="A102" r:id="rId105" xr:uid="{A059E2A8-5585-7B46-B48E-443BA07775B4}"/>
+    <hyperlink ref="A104" r:id="rId106" xr:uid="{1284E9E2-0FC0-F943-B176-5B97E54132B8}"/>
+    <hyperlink ref="A106" r:id="rId107" xr:uid="{8E654989-AEEC-FF4C-89F0-951B5DCFF5D3}"/>
+    <hyperlink ref="A108" r:id="rId108" xr:uid="{C82CDCF7-522C-E94B-9C53-A41F4BDA6870}"/>
+    <hyperlink ref="A110" r:id="rId109" xr:uid="{A268274E-EB3F-6B47-AD58-F48D17E13A01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>